<commit_message>
edit - edit image logo
</commit_message>
<xml_diff>
--- a/tem_data.xlsx
+++ b/tem_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\recursoiglesia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB17555-1E3D-48CB-9A5C-9104B6D8A44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92911F3-B555-4827-A94B-49FDBA998E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9349,10 +9349,17 @@
   <dimension ref="A1:E601"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="121.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.69921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>